<commit_message>
update: excel date update
</commit_message>
<xml_diff>
--- a/test/official_test_case_1.xlsx
+++ b/test/official_test_case_1.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Intern\WEHI\prod\forecasting-with-workday-project\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBE241E-1D04-46EC-8E83-46641D33F279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C03C37-189C-4059-BB2D-6495D001B5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Funding" sheetId="1" r:id="rId1"/>
-    <sheet name="Expense" sheetId="2" r:id="rId2"/>
+    <sheet name="Description" sheetId="3" r:id="rId1"/>
+    <sheet name="Funding" sheetId="1" r:id="rId2"/>
+    <sheet name="Expense" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
   <si>
     <t>Source ID</t>
   </si>
@@ -201,9 +202,6 @@
   </si>
   <si>
     <t>E010</t>
-  </si>
-  <si>
-    <t>sam</t>
   </si>
 </sst>
 </file>
@@ -261,6 +259,135 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63905A52-F4D6-49DF-BEB7-EE3905BCD1F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="167640" y="220980"/>
+          <a:ext cx="3657600" cy="901700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>What’s happening:</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Funding and expenses line up well across time and categories, so nothing blocks allocation. Salary fund </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AE"/>
+            <a:t>₹20</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>k + Salary expense </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AE"/>
+            <a:t>₹10</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>k - fully covered</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Equipment fund </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AE"/>
+            <a:t>₹15</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>k + Equipment expense </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AE"/>
+            <a:t>₹12</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>k - fully covered</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> Everything connects cleanly, no leftovers cause issues.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -541,6 +668,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF27846-F087-4848-B7B4-26D7FF40435C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
@@ -883,15 +1025,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C11"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -924,7 +1069,7 @@
         <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -944,7 +1089,7 @@
         <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -964,7 +1109,7 @@
         <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
@@ -984,7 +1129,7 @@
         <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -1004,7 +1149,7 @@
         <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -1024,7 +1169,7 @@
         <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
@@ -1044,7 +1189,7 @@
         <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -1064,7 +1209,7 @@
         <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
@@ -1084,7 +1229,7 @@
         <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
@@ -1104,7 +1249,7 @@
         <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>

</xml_diff>